<commit_message>
Added database file column
</commit_message>
<xml_diff>
--- a/EnvNP_Philippines.xlsx
+++ b/EnvNP_Philippines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvvvvv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4473BAD3-780D-7146-8845-6FB49FBAC00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E6EC60-563E-A047-B076-089B54BBCFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="980" windowWidth="27640" windowHeight="15320" xr2:uid="{D65F6AAF-E950-4849-92E2-13DA499F7162}"/>
+    <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15320" xr2:uid="{D65F6AAF-E950-4849-92E2-13DA499F7162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
   <si>
     <t>Society for the Conservation of Philippine Wetlands, Inc.</t>
   </si>
@@ -385,6 +385,36 @@
     <t>- Fundraisers
 - Corporate partnerships
 - Donations</t>
+  </si>
+  <si>
+    <t>Name of organisation</t>
+  </si>
+  <si>
+    <t>Description of organisation</t>
+  </si>
+  <si>
+    <t>Mission/ Objectives/ Purpose</t>
+  </si>
+  <si>
+    <t>Programmes/ projects</t>
+  </si>
+  <si>
+    <t>Funding sources</t>
+  </si>
+  <si>
+    <t>Collaboration with government / businesses</t>
+  </si>
+  <si>
+    <t>Choice of Climate action</t>
+  </si>
+  <si>
+    <t>No. of employees</t>
+  </si>
+  <si>
+    <t>Geographical focus</t>
+  </si>
+  <si>
+    <t>Nationality</t>
   </si>
 </sst>
 </file>
@@ -420,12 +450,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -440,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -449,6 +485,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -765,70 +804,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EE165F-363D-604D-A29D-558CAC6D08F6}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
+    <row r="1" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -837,65 +876,65 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="307" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="307" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
@@ -903,28 +942,28 @@
     </row>
     <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
+      <c r="H5" s="2">
+        <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>7</v>
@@ -935,28 +974,28 @@
     </row>
     <row r="6" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>7</v>
@@ -967,28 +1006,28 @@
     </row>
     <row r="7" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>7</v>
@@ -997,65 +1036,65 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="294" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="294" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="2">
-        <v>33</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>8</v>
@@ -1063,31 +1102,31 @@
     </row>
     <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
+      <c r="H10" s="2">
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>8</v>
@@ -1095,90 +1134,90 @@
     </row>
     <row r="11" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="2">
-        <v>9</v>
-      </c>
-      <c r="I11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="2">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>7</v>
@@ -1187,30 +1226,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="197" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="2">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>7</v>
@@ -1219,30 +1258,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="281" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="197" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>82</v>
+      <c r="H15" s="2">
+        <v>46</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>7</v>
@@ -1251,30 +1290,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="281" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="2">
-        <v>53</v>
+      <c r="H16" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>7</v>
@@ -1283,24 +1322,56 @@
         <v>8</v>
       </c>
     </row>
+    <row r="17" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2">
+        <v>53</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A16" r:id="rId1" xr:uid="{D5BDA802-2A55-634C-AF8B-CB580E31852A}"/>
-    <hyperlink ref="A15" r:id="rId2" xr:uid="{CC06DFFD-1710-C540-986E-A2EA540CFA93}"/>
-    <hyperlink ref="A14" r:id="rId3" xr:uid="{1EF58631-58B7-8A48-99A5-DA7966EB00FE}"/>
-    <hyperlink ref="A13" r:id="rId4" xr:uid="{C66ED768-5EB4-594E-82D5-5325DA355EE9}"/>
-    <hyperlink ref="A12" r:id="rId5" xr:uid="{63E35546-4AA4-C348-94A9-160857B412B2}"/>
-    <hyperlink ref="A11" r:id="rId6" xr:uid="{F6D3F864-0E29-3149-A75C-5030450532CB}"/>
-    <hyperlink ref="A10" r:id="rId7" xr:uid="{85D25AB6-D764-8A46-8943-ED28A31F1C9C}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{E5FE6F7B-26CB-ED42-8D47-5C3553B321C3}"/>
-    <hyperlink ref="A8" r:id="rId9" xr:uid="{8A900642-50AA-6844-9942-D09D3401097A}"/>
-    <hyperlink ref="A7" r:id="rId10" xr:uid="{8D63A223-3A83-DD46-BC10-6259633A2C91}"/>
-    <hyperlink ref="A6" r:id="rId11" xr:uid="{6E78FAA6-C5C4-0849-AB80-6D5EF790AE6E}"/>
-    <hyperlink ref="A5" r:id="rId12" xr:uid="{8FE48755-E4B6-EC47-B241-5754CA612597}"/>
-    <hyperlink ref="A4" r:id="rId13" xr:uid="{3F6D14B2-9750-CA42-9FA9-3065F36ED18B}"/>
-    <hyperlink ref="A3" r:id="rId14" xr:uid="{F18C3116-F936-114E-BE70-C5FCF5234B15}"/>
-    <hyperlink ref="A2" r:id="rId15" xr:uid="{5FA219F5-B761-3045-AB7D-A97E999DDE22}"/>
-    <hyperlink ref="A1" r:id="rId16" xr:uid="{CBE0A598-C3AB-4440-8C71-463F3B8942F1}"/>
+    <hyperlink ref="A17" r:id="rId1" xr:uid="{D5BDA802-2A55-634C-AF8B-CB580E31852A}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{CC06DFFD-1710-C540-986E-A2EA540CFA93}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{1EF58631-58B7-8A48-99A5-DA7966EB00FE}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{C66ED768-5EB4-594E-82D5-5325DA355EE9}"/>
+    <hyperlink ref="A13" r:id="rId5" xr:uid="{63E35546-4AA4-C348-94A9-160857B412B2}"/>
+    <hyperlink ref="A12" r:id="rId6" xr:uid="{F6D3F864-0E29-3149-A75C-5030450532CB}"/>
+    <hyperlink ref="A11" r:id="rId7" xr:uid="{85D25AB6-D764-8A46-8943-ED28A31F1C9C}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{E5FE6F7B-26CB-ED42-8D47-5C3553B321C3}"/>
+    <hyperlink ref="A9" r:id="rId9" xr:uid="{8A900642-50AA-6844-9942-D09D3401097A}"/>
+    <hyperlink ref="A8" r:id="rId10" xr:uid="{8D63A223-3A83-DD46-BC10-6259633A2C91}"/>
+    <hyperlink ref="A7" r:id="rId11" xr:uid="{6E78FAA6-C5C4-0849-AB80-6D5EF790AE6E}"/>
+    <hyperlink ref="A6" r:id="rId12" xr:uid="{8FE48755-E4B6-EC47-B241-5754CA612597}"/>
+    <hyperlink ref="A5" r:id="rId13" xr:uid="{3F6D14B2-9750-CA42-9FA9-3065F36ED18B}"/>
+    <hyperlink ref="A4" r:id="rId14" xr:uid="{F18C3116-F936-114E-BE70-C5FCF5234B15}"/>
+    <hyperlink ref="A3" r:id="rId15" xr:uid="{5FA219F5-B761-3045-AB7D-A97E999DDE22}"/>
+    <hyperlink ref="A2" r:id="rId16" xr:uid="{CBE0A598-C3AB-4440-8C71-463F3B8942F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>